<commit_message>
03.09.2020 M C Details
</commit_message>
<xml_diff>
--- a/2020/August/All Detail/31.08.2020/MC Balance Transfer August 2020.xlsx
+++ b/2020/August/All Detail/31.08.2020/MC Balance Transfer August 2020.xlsx
@@ -1117,7 +1117,7 @@
         <xdr:cNvPr id="1317" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AEF7B42F-C37B-44F8-8D5A-2ED7FEE15E8A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEF7B42F-C37B-44F8-8D5A-2ED7FEE15E8A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1129,7 +1129,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1152,14 +1152,14 @@
         </a:ln>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -1467,9 +1467,9 @@
   <dimension ref="A1:BI231"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="4" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="I1" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="G99" sqref="G99"/>
+      <selection pane="bottomLeft" activeCell="I54" sqref="I54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -4050,11 +4050,11 @@
       </c>
       <c r="E36" s="114">
         <f>F33-C98+K121</f>
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="F36" s="63">
         <f>F33-C98-I43-I42+K121-C103</f>
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="G36" s="81"/>
       <c r="H36" s="86"/>
@@ -5143,7 +5143,7 @@
       </c>
       <c r="B52" s="70"/>
       <c r="C52" s="134">
-        <v>164630</v>
+        <v>154630</v>
       </c>
       <c r="D52" s="128" t="s">
         <v>90</v>
@@ -8467,7 +8467,7 @@
       <c r="B98" s="146"/>
       <c r="C98" s="32">
         <f>SUM(C37:C97)</f>
-        <v>1474832</v>
+        <v>1464832</v>
       </c>
       <c r="D98" s="28"/>
       <c r="F98" s="110"/>
@@ -8602,7 +8602,7 @@
       <c r="B100" s="144"/>
       <c r="C100" s="29">
         <f>C98+L121</f>
-        <v>1474832</v>
+        <v>1464832</v>
       </c>
       <c r="D100" s="21"/>
       <c r="F100" s="48"/>

</xml_diff>